<commit_message>
File updated with geeksforgeeks python basic file.direc operations
</commit_message>
<xml_diff>
--- a/Python.xlsx
+++ b/Python.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27715"/>
+  <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Rao/Programming/python/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500"/>
   </bookViews>
   <sheets>
     <sheet name="Data Types" sheetId="1" r:id="rId1"/>
@@ -16,12 +21,20 @@
     <sheet name="regex" sheetId="8" r:id="rId7"/>
     <sheet name="file" sheetId="9" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="135">
   <si>
     <t>Tuple</t>
   </si>
@@ -423,13 +436,16 @@
   </si>
   <si>
     <t>index or error</t>
+  </si>
+  <si>
+    <t>http://www.geeksforgeeks.org/listing-directories-files-python/?utm_source=feedburner&amp;utm_medium=email&amp;utm_campaign=Feed%3A+Geeksforgeeks+%28GeeksforGeeks%29</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -479,6 +495,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -525,12 +546,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -557,14 +578,15 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -591,6 +613,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -766,22 +789,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B5:F10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B5:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" customWidth="1"/>
-    <col min="5" max="5" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="51.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" customWidth="1"/>
+    <col min="5" max="5" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:6">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
@@ -798,7 +821,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:6">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>0</v>
       </c>
@@ -815,12 +838,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="2:6">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
       <c r="F7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="2:6">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>2</v>
       </c>
@@ -834,12 +857,17 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="2:6">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>104</v>
       </c>
       <c r="D10" t="s">
         <v>105</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -849,22 +877,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>24</v>
@@ -876,7 +904,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>15</v>
       </c>
@@ -887,7 +915,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>33</v>
       </c>
@@ -901,32 +929,32 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>108</v>
       </c>
@@ -937,7 +965,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>110</v>
       </c>
@@ -945,12 +973,12 @@
         <v>112</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>114</v>
       </c>
@@ -961,25 +989,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="2:4">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>42</v>
       </c>
@@ -990,7 +1018,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="2:4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>41</v>
       </c>
@@ -1001,7 +1029,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="2:4">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>47</v>
       </c>
@@ -1012,7 +1040,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="2:4">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>50</v>
       </c>
@@ -1023,7 +1051,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="2:4">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>52</v>
       </c>
@@ -1034,7 +1062,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="2:4">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>48</v>
       </c>
@@ -1051,26 +1079,26 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="1" customFormat="1">
+    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>65</v>
       </c>
@@ -1084,7 +1112,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>29</v>
       </c>
@@ -1095,17 +1123,17 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>35</v>
       </c>
@@ -1116,7 +1144,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C9" s="2" t="s">
         <v>36</v>
       </c>
@@ -1124,7 +1152,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C10" s="2" t="s">
         <v>27</v>
       </c>
@@ -1132,7 +1160,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>61</v>
       </c>
@@ -1143,7 +1171,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C13" s="2" t="s">
         <v>36</v>
       </c>
@@ -1151,7 +1179,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C14" s="2" t="s">
         <v>27</v>
       </c>
@@ -1159,7 +1187,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>56</v>
       </c>
@@ -1179,21 +1207,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>78</v>
       </c>
@@ -1201,7 +1229,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="1" customFormat="1">
+    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>65</v>
       </c>
@@ -1215,7 +1243,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>28</v>
       </c>
@@ -1229,7 +1257,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>26</v>
       </c>
@@ -1240,12 +1268,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>57</v>
       </c>
@@ -1256,7 +1284,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>22</v>
       </c>
@@ -1267,17 +1295,17 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>117</v>
       </c>
@@ -1288,12 +1316,12 @@
         <v>133</v>
       </c>
     </row>
-    <row r="17" spans="3:3">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="3:3">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
         <v>86</v>
       </c>
@@ -1305,19 +1333,19 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
         <v>66</v>
       </c>
@@ -1325,7 +1353,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="2:5">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>19</v>
       </c>
@@ -1336,7 +1364,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="2:5">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
         <v>63</v>
       </c>
@@ -1344,7 +1372,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="2:5">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
         <v>64</v>
       </c>
@@ -1352,7 +1380,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="2:5">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
         <v>67</v>
       </c>
@@ -1360,7 +1388,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="2:5">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
         <v>130</v>
       </c>
@@ -1368,7 +1396,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="12" spans="2:5">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E12" t="s">
         <v>132</v>
       </c>
@@ -1379,20 +1407,20 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="21.42578125" customWidth="1"/>
-    <col min="6" max="6" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5" customWidth="1"/>
+    <col min="6" max="6" width="27.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:6" s="1" customFormat="1">
+    <row r="4" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C4" s="1" t="s">
         <v>72</v>
       </c>
@@ -1406,7 +1434,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="2:6">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>34</v>
       </c>
@@ -1423,7 +1451,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="2:6">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D6" t="s">
         <v>75</v>
       </c>
@@ -1431,7 +1459,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="8" spans="2:6">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
         <v>73</v>
       </c>
@@ -1445,7 +1473,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="2:6">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D9" t="s">
         <v>75</v>
       </c>
@@ -1453,12 +1481,12 @@
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="2:6">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D10" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="2:6">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
         <v>100</v>
       </c>
@@ -1472,7 +1500,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="2:6">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D13" t="s">
         <v>75</v>
       </c>
@@ -1480,7 +1508,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="14" spans="2:6">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D14" t="s">
         <v>98</v>
       </c>
@@ -1491,16 +1519,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="3" spans="2:7">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>118</v>
       </c>
@@ -1514,7 +1542,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="2:7">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>119</v>
       </c>
@@ -1522,7 +1550,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="2:7">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>122</v>
       </c>
@@ -1530,7 +1558,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="8" spans="2:7">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>123</v>
       </c>
@@ -1538,7 +1566,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="10" spans="2:7">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>128</v>
       </c>

</xml_diff>